<commit_message>
Arborescence modification + Additional datasets
</commit_message>
<xml_diff>
--- a/IEC/D-IEC/M-IEC/Anisimov2014.xlsx
+++ b/IEC/D-IEC/M-IEC/Anisimov2014.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZ\alaniszeo_git\EC-generic-model\Database_for_model_validation\M-IEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZ\alaniszeo_git\OSD-ECMTest\IEC\D-IEC\M-IEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32531552-7224-4539-BAC6-CED1E5489CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F2B9B3-0936-402A-A2E0-33293AD2308E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{1306219A-737B-4B5D-BCFD-98C34D3C77CC}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1306219A-737B-4B5D-BCFD-98C34D3C77CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Anisimov2014" sheetId="8" r:id="rId1"/>
@@ -630,6 +630,12 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -638,12 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8574891-75AC-4FF0-A209-A0439F96762A}">
   <dimension ref="B1:AC134"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1140,7 @@
       <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="70">
+      <c r="C5" s="67">
         <v>2014</v>
       </c>
       <c r="N5" s="6"/>
@@ -1155,23 +1155,23 @@
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="2:14" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="70"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9613,8 +9613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86117A86-B0AF-4F7B-BAC5-84FF1326045A}">
   <dimension ref="B1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A22" zoomScale="104" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9697,23 +9697,23 @@
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="2:14" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="70"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>